<commit_message>
original test is fine
</commit_message>
<xml_diff>
--- a/testData/bdor_test.xlsx
+++ b/testData/bdor_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F74DF-BAB5-EE4B-A85B-44976F2FB0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C12FE-0F60-6D48-BEAC-D8F4EDA774C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35420" yWindow="-21100" windowWidth="19200" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$CH$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$CH$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="114">
   <si>
     <t>計劃單號</t>
   </si>
@@ -379,16 +379,7 @@
     <t xml:space="preserve">TAC11154940       </t>
   </si>
   <si>
-    <t xml:space="preserve">TAC00066440       </t>
-  </si>
-  <si>
     <t>10/26/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/24/23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAC11187850       </t>
   </si>
 </sst>
 </file>
@@ -839,12 +830,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:CH36"/>
+  <dimension ref="A1:CH33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="W1" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="W24" sqref="W24"/>
+      <selection pane="bottomLeft" activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,7 +1168,7 @@
     </row>
     <row r="3" spans="1:86" hidden="1" x14ac:dyDescent="0.2">
       <c r="W3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y3" s="7" t="s">
         <v>96</v>
@@ -1195,7 +1186,7 @@
     </row>
     <row r="4" spans="1:86" hidden="1" x14ac:dyDescent="0.2">
       <c r="W4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>96</v>
@@ -1525,9 +1516,9 @@
         <v>36.31</v>
       </c>
     </row>
-    <row r="22" spans="23:54" x14ac:dyDescent="0.2">
+    <row r="22" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="W22" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y22" s="7" t="s">
         <v>103</v>
@@ -1543,9 +1534,9 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="23:54" x14ac:dyDescent="0.2">
+    <row r="23" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="W23" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y23" s="7" t="s">
         <v>103</v>
@@ -1561,7 +1552,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="24" spans="23:54" x14ac:dyDescent="0.2">
+    <row r="24" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="W24" s="3">
         <v>45232</v>
       </c>
@@ -1579,7 +1570,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="25" spans="23:54" x14ac:dyDescent="0.2">
+    <row r="25" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="W25" s="3">
         <v>45232</v>
       </c>
@@ -1725,53 +1716,11 @@
         <v>406.89</v>
       </c>
     </row>
-    <row r="34" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
-      <c r="W34" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>113</v>
-      </c>
-      <c r="AQ34">
-        <v>0.13</v>
-      </c>
-      <c r="BB34">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="35" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
-      <c r="W35" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ35">
-        <v>57.816000000000003</v>
-      </c>
-      <c r="BB35">
-        <v>57.82</v>
-      </c>
-    </row>
-    <row r="36" spans="23:54" hidden="1" x14ac:dyDescent="0.2">
-      <c r="W36" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ36">
-        <v>14.436</v>
-      </c>
-      <c r="BB36">
-        <v>14.44</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:CH36" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:CH33" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="24">
       <filters>
-        <filter val="TAC11181440"/>
+        <filter val="TAC00066440"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>